<commit_message>
Moved templates and static folders to icss-backend
</commit_message>
<xml_diff>
--- a/RPN.xlsx
+++ b/RPN.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lakshya\Project\ICSS_VSCode\PROJECT\ProcessedData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KOEL\ICSS\Deployment\icss-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7A2F25-1E43-4744-A91D-6B96B1F09BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7845"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -608,7 +609,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -936,23 +937,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F186"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
@@ -972,7 +973,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -992,7 +993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1012,7 +1013,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1032,7 +1033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1052,7 +1053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1072,7 +1073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1092,7 +1093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1112,7 +1113,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1132,7 +1133,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1152,7 +1153,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1172,7 +1173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1192,7 +1193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -1212,7 +1213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1232,7 +1233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1252,7 +1253,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1272,7 +1273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1292,7 +1293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1312,7 +1313,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1332,7 +1333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1352,7 +1353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1372,7 +1373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1392,7 +1393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1412,7 +1413,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
@@ -1452,7 +1453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
@@ -1472,7 +1473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
@@ -1492,7 +1493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
@@ -1512,7 +1513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
@@ -1532,7 +1533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
@@ -1552,7 +1553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
@@ -1572,7 +1573,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
@@ -1592,7 +1593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -1612,7 +1613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>80</v>
       </c>
@@ -1632,7 +1633,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>81</v>
       </c>
@@ -1652,7 +1653,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>82</v>
       </c>
@@ -1672,7 +1673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>83</v>
       </c>
@@ -1692,7 +1693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>84</v>
       </c>
@@ -1712,7 +1713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>85</v>
       </c>
@@ -1732,7 +1733,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>37</v>
       </c>
@@ -1752,7 +1753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>38</v>
       </c>
@@ -1772,7 +1773,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>39</v>
       </c>
@@ -1792,7 +1793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>86</v>
       </c>
@@ -1812,7 +1813,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>87</v>
       </c>
@@ -1832,7 +1833,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>88</v>
       </c>
@@ -1852,7 +1853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>89</v>
       </c>
@@ -1872,7 +1873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>90</v>
       </c>
@@ -1892,7 +1893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>91</v>
       </c>
@@ -1912,7 +1913,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>92</v>
       </c>
@@ -1932,7 +1933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>93</v>
       </c>
@@ -1952,7 +1953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>94</v>
       </c>
@@ -1972,7 +1973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>95</v>
       </c>
@@ -1992,7 +1993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>96</v>
       </c>
@@ -2012,7 +2013,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>97</v>
       </c>
@@ -2032,7 +2033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>98</v>
       </c>
@@ -2052,7 +2053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>99</v>
       </c>
@@ -2072,7 +2073,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>100</v>
       </c>
@@ -2092,7 +2093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>101</v>
       </c>
@@ -2112,7 +2113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>40</v>
       </c>
@@ -2132,7 +2133,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>41</v>
       </c>
@@ -2152,7 +2153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>102</v>
       </c>
@@ -2172,7 +2173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>103</v>
       </c>
@@ -2192,7 +2193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>104</v>
       </c>
@@ -2212,7 +2213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>105</v>
       </c>
@@ -2232,7 +2233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>106</v>
       </c>
@@ -2252,7 +2253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>107</v>
       </c>
@@ -2272,7 +2273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>43</v>
       </c>
@@ -2292,7 +2293,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>44</v>
       </c>
@@ -2312,7 +2313,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>45</v>
       </c>
@@ -2332,7 +2333,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>108</v>
       </c>
@@ -2352,7 +2353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>46</v>
       </c>
@@ -2372,7 +2373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>47</v>
       </c>
@@ -2392,7 +2393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>48</v>
       </c>
@@ -2412,7 +2413,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>49</v>
       </c>
@@ -2432,7 +2433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>50</v>
       </c>
@@ -2452,7 +2453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>51</v>
       </c>
@@ -2472,7 +2473,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>109</v>
       </c>
@@ -2492,7 +2493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>54</v>
       </c>
@@ -2512,7 +2513,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>52</v>
       </c>
@@ -2532,7 +2533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>110</v>
       </c>
@@ -2552,7 +2553,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>53</v>
       </c>
@@ -2572,7 +2573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>55</v>
       </c>
@@ -2592,7 +2593,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>111</v>
       </c>
@@ -2612,7 +2613,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>112</v>
       </c>
@@ -2632,7 +2633,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>113</v>
       </c>
@@ -2652,7 +2653,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>114</v>
       </c>
@@ -2672,7 +2673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>115</v>
       </c>
@@ -2692,7 +2693,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>116</v>
       </c>
@@ -2712,7 +2713,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>117</v>
       </c>
@@ -2732,7 +2733,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>56</v>
       </c>
@@ -2752,7 +2753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>57</v>
       </c>
@@ -2772,7 +2773,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>58</v>
       </c>
@@ -2792,7 +2793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>118</v>
       </c>
@@ -2812,7 +2813,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>59</v>
       </c>
@@ -2832,7 +2833,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>60</v>
       </c>
@@ -2852,7 +2853,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>61</v>
       </c>
@@ -2872,7 +2873,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>62</v>
       </c>
@@ -2892,7 +2893,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>119</v>
       </c>
@@ -2912,7 +2913,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>120</v>
       </c>
@@ -2932,7 +2933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>121</v>
       </c>
@@ -2952,7 +2953,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>122</v>
       </c>
@@ -2972,7 +2973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>123</v>
       </c>
@@ -2992,7 +2993,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>124</v>
       </c>
@@ -3012,7 +3013,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>125</v>
       </c>
@@ -3032,7 +3033,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>126</v>
       </c>
@@ -3052,7 +3053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>127</v>
       </c>
@@ -3072,7 +3073,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>128</v>
       </c>
@@ -3092,7 +3093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>129</v>
       </c>
@@ -3112,7 +3113,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>130</v>
       </c>
@@ -3132,7 +3133,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>131</v>
       </c>
@@ -3152,7 +3153,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>132</v>
       </c>
@@ -3172,7 +3173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>133</v>
       </c>
@@ -3192,7 +3193,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>134</v>
       </c>
@@ -3212,7 +3213,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>135</v>
       </c>
@@ -3232,7 +3233,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>136</v>
       </c>
@@ -3252,7 +3253,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>137</v>
       </c>
@@ -3272,7 +3273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>138</v>
       </c>
@@ -3292,7 +3293,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>139</v>
       </c>
@@ -3312,7 +3313,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>140</v>
       </c>
@@ -3332,7 +3333,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>141</v>
       </c>
@@ -3352,7 +3353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>142</v>
       </c>
@@ -3372,7 +3373,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>143</v>
       </c>
@@ -3392,7 +3393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>63</v>
       </c>
@@ -3412,7 +3413,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>65</v>
       </c>
@@ -3432,7 +3433,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>66</v>
       </c>
@@ -3452,7 +3453,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>67</v>
       </c>
@@ -3472,7 +3473,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>68</v>
       </c>
@@ -3492,7 +3493,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>69</v>
       </c>
@@ -3512,7 +3513,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>70</v>
       </c>
@@ -3532,7 +3533,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>71</v>
       </c>
@@ -3552,7 +3553,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>72</v>
       </c>
@@ -3572,7 +3573,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>73</v>
       </c>
@@ -3592,7 +3593,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>74</v>
       </c>
@@ -3612,7 +3613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>75</v>
       </c>
@@ -3632,7 +3633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>76</v>
       </c>
@@ -3652,7 +3653,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>144</v>
       </c>
@@ -3672,7 +3673,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>145</v>
       </c>
@@ -3692,7 +3693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>146</v>
       </c>
@@ -3712,7 +3713,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>147</v>
       </c>
@@ -3732,7 +3733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>148</v>
       </c>
@@ -3752,7 +3753,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>149</v>
       </c>
@@ -3772,7 +3773,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>150</v>
       </c>
@@ -3792,7 +3793,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>151</v>
       </c>
@@ -3812,7 +3813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>152</v>
       </c>
@@ -3832,7 +3833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>153</v>
       </c>
@@ -3852,7 +3853,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>154</v>
       </c>
@@ -3872,7 +3873,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>155</v>
       </c>
@@ -3892,7 +3893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>156</v>
       </c>
@@ -3912,7 +3913,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>157</v>
       </c>
@@ -3932,7 +3933,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>158</v>
       </c>
@@ -3952,7 +3953,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>159</v>
       </c>
@@ -3972,7 +3973,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>160</v>
       </c>
@@ -3992,7 +3993,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>42</v>
       </c>
@@ -4012,7 +4013,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>161</v>
       </c>
@@ -4032,7 +4033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>120</v>
       </c>
@@ -4052,7 +4053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>162</v>
       </c>
@@ -4072,7 +4073,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>163</v>
       </c>
@@ -4092,7 +4093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>126</v>
       </c>
@@ -4112,7 +4113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>164</v>
       </c>
@@ -4132,7 +4133,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>166</v>
       </c>
@@ -4152,7 +4153,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>167</v>
       </c>
@@ -4172,7 +4173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>168</v>
       </c>
@@ -4192,7 +4193,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>169</v>
       </c>
@@ -4212,7 +4213,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>171</v>
       </c>
@@ -4232,7 +4233,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>172</v>
       </c>
@@ -4252,7 +4253,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>173</v>
       </c>
@@ -4272,7 +4273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>174</v>
       </c>
@@ -4292,7 +4293,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>165</v>
       </c>
@@ -4312,7 +4313,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>175</v>
       </c>
@@ -4332,7 +4333,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>176</v>
       </c>
@@ -4352,7 +4353,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>177</v>
       </c>
@@ -4372,7 +4373,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>178</v>
       </c>
@@ -4392,7 +4393,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>179</v>
       </c>
@@ -4412,7 +4413,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>180</v>
       </c>
@@ -4432,7 +4433,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>181</v>
       </c>
@@ -4452,7 +4453,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>182</v>
       </c>
@@ -4472,7 +4473,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>183</v>
       </c>
@@ -4492,7 +4493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>184</v>
       </c>
@@ -4512,7 +4513,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>185</v>
       </c>
@@ -4532,7 +4533,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>186</v>
       </c>
@@ -4552,7 +4553,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>187</v>
       </c>
@@ -4572,7 +4573,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>188</v>
       </c>
@@ -4592,7 +4593,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>189</v>
       </c>
@@ -4612,7 +4613,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>190</v>
       </c>
@@ -4632,7 +4633,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>191</v>
       </c>
@@ -4652,7 +4653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>192</v>
       </c>

</xml_diff>